<commit_message>
register uploaded image momdel to admin site
</commit_message>
<xml_diff>
--- a/Requirement_Traceability_Matrix.xlsx
+++ b/Requirement_Traceability_Matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevd\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevd\OneDrive\Documents\capstone_UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7099D89-2549-4BAB-A776-9228AE3A3FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C8E466-00B4-439C-BF9C-BBE36A51E46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F6F66CB-27E2-49A5-990C-7DFD9CA5579F}"/>
   </bookViews>
@@ -233,14 +233,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -290,14 +289,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F6" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8384FB66-56FA-48BE-BE64-882EF2D985BB}" name="Report Section" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F965AAFA-1C00-4543-93FC-28AD46D0245A}" name="Name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F6DA9492-CDDB-4753-8E1F-81D9009A5E9E}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{E8E6DE19-837D-4AD6-BB88-8B7F0533BC3D}" name="Feature Specification" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{75DA1F04-D729-4AD5-B1C8-98B285782BD2}" name="Reference" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8384FB66-56FA-48BE-BE64-882EF2D985BB}" name="Report Section" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F965AAFA-1C00-4543-93FC-28AD46D0245A}" name="Name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6DA9492-CDDB-4753-8E1F-81D9009A5E9E}" name="Description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E8E6DE19-837D-4AD6-BB88-8B7F0533BC3D}" name="Feature Specification" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{75DA1F04-D729-4AD5-B1C8-98B285782BD2}" name="Reference" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{E16B3242-CE4B-4B92-8D3C-07721D99D275}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -769,7 +768,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -793,7 +792,7 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -806,7 +805,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="F9" t="s">
@@ -841,8 +840,8 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to notes and excel
</commit_message>
<xml_diff>
--- a/Requirement_Traceability_Matrix.xlsx
+++ b/Requirement_Traceability_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevd\OneDrive\Documents\capstone_UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C8E466-00B4-439C-BF9C-BBE36A51E46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949E3668-5BE6-4A98-BAD6-FC1FB1EA9E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F6F66CB-27E2-49A5-990C-7DFD9CA5579F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Report Section</t>
   </si>
@@ -171,17 +171,38 @@
     <t>A standard user (healthcare professional) and admin user (one who can register users)</t>
   </si>
   <si>
-    <t>Check HL7 for anything on this type of administration</t>
-  </si>
-  <si>
     <t>Current Edition (dicomstandard.org)</t>
+  </si>
+  <si>
+    <t>custom session store or 3rd party application</t>
+  </si>
+  <si>
+    <t>pydicom</t>
+  </si>
+  <si>
+    <t>hl7apy,python-hl7</t>
+  </si>
+  <si>
+    <t>fhir.resources, fhirclient, PyFHIR</t>
+  </si>
+  <si>
+    <t>Pairs metadata with pixel data into a .dcm file format, a medical standard, ISO 12052:2017</t>
+  </si>
+  <si>
+    <t>Modern HL7 using RESTful APIs</t>
+  </si>
+  <si>
+    <t>Standard for exchanging electronic health care data, using an older messaging approach</t>
+  </si>
+  <si>
+    <t>Django can do this, except multi-tenancy needs a package</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +232,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -233,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -289,15 +318,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F6" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:F9" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8384FB66-56FA-48BE-BE64-882EF2D985BB}" name="Report Section" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F965AAFA-1C00-4543-93FC-28AD46D0245A}" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F6DA9492-CDDB-4753-8E1F-81D9009A5E9E}" name="Description" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E8E6DE19-837D-4AD6-BB88-8B7F0533BC3D}" name="Feature Specification" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{75DA1F04-D729-4AD5-B1C8-98B285782BD2}" name="Reference" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{E16B3242-CE4B-4B92-8D3C-07721D99D275}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8384FB66-56FA-48BE-BE64-882EF2D985BB}" name="Report Section" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F965AAFA-1C00-4543-93FC-28AD46D0245A}" name="Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F6DA9492-CDDB-4753-8E1F-81D9009A5E9E}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E8E6DE19-837D-4AD6-BB88-8B7F0533BC3D}" name="Feature Specification" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{75DA1F04-D729-4AD5-B1C8-98B285782BD2}" name="Reference" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{E16B3242-CE4B-4B92-8D3C-07721D99D275}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -620,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7F718F-2F7A-4F5E-9A03-E4EADA47E05A}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +702,9 @@
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -740,7 +771,55 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +836,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,7 +915,7 @@
         <v>37</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
time to go to school
</commit_message>
<xml_diff>
--- a/Requirement_Traceability_Matrix.xlsx
+++ b/Requirement_Traceability_Matrix.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevd\OneDrive\Documents\capstone_UI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevd\OneDrive\Desktop\Projects\capstone_UI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524D4E92-DD4C-466D-8E34-6F5A4AFEABFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6971C616-3506-42F8-B68A-2E735A3BBE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4F6F66CB-27E2-49A5-990C-7DFD9CA5579F}"/>
+    <workbookView xWindow="28710" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4F6F66CB-27E2-49A5-990C-7DFD9CA5579F}"/>
   </bookViews>
   <sheets>
     <sheet name="Traceability Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="Legal Compliance" sheetId="2" r:id="rId2"/>
-    <sheet name="PIPEDA" sheetId="3" r:id="rId3"/>
-    <sheet name="Privacy Act" sheetId="4" r:id="rId4"/>
-    <sheet name="Personal Information Protection" sheetId="5" r:id="rId5"/>
+    <sheet name="Data Privacy and Security Guide" sheetId="6" r:id="rId3"/>
+    <sheet name="Notes" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
   <si>
     <t>Report Section</t>
   </si>
@@ -60,45 +59,21 @@
     <t>3.2.4</t>
   </si>
   <si>
-    <t>Image Storage</t>
-  </si>
-  <si>
-    <t>The retention period for patient data (fundus images in our case)</t>
-  </si>
-  <si>
     <t>HTTPS</t>
   </si>
   <si>
     <t>Encryption for data in transit</t>
   </si>
   <si>
-    <t>Delete image from storage system after its been used for a report. Otherwise, remove after the session ends.</t>
-  </si>
-  <si>
     <t>Use the HTTPS protocol for communication</t>
   </si>
   <si>
     <t>3.2.6</t>
   </si>
   <si>
-    <t>PIPEDA Compliance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comply with PIPEDA legislation on </t>
   </si>
   <si>
-    <t>PIPEDA, Principle #5, "</t>
-  </si>
-  <si>
-    <t>Each principle needs to be complied with</t>
-  </si>
-  <si>
-    <t>https://www.priv.gc.ca/en/privacy-topics/privacy-laws-in-canada/the-personal-information-protection-and-electronic-documents-act-pipeda/r_o_p/prov-pipeda/</t>
-  </si>
-  <si>
-    <t>Generally exempt from PIPEDA given the private-sectory privacy laws</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -177,27 +152,9 @@
     <t>Current Edition (dicomstandard.org)</t>
   </si>
   <si>
-    <t>custom session store or 3rd party application</t>
-  </si>
-  <si>
     <t>pydicom</t>
   </si>
   <si>
-    <t>hl7apy,python-hl7</t>
-  </si>
-  <si>
-    <t>fhir.resources, fhirclient, PyFHIR</t>
-  </si>
-  <si>
-    <t>Pairs metadata with pixel data into a .dcm file format, a medical standard, ISO 12052:2017</t>
-  </si>
-  <si>
-    <t>Modern HL7 using RESTful APIs</t>
-  </si>
-  <si>
-    <t>Standard for exchanging electronic health care data, using an older messaging approach</t>
-  </si>
-  <si>
     <t>Django can do this, except multi-tenancy needs a package</t>
   </si>
   <si>
@@ -225,18 +182,12 @@
     <t>What that means for us</t>
   </si>
   <si>
-    <t>Remove PHI once it is used</t>
-  </si>
-  <si>
     <t>A section in the user guide or other documentation</t>
   </si>
   <si>
     <t>If we ever choose to send or receive PHI then it is applicable</t>
   </si>
   <si>
-    <t>IDK</t>
-  </si>
-  <si>
     <t>Principle 3 - Consent</t>
   </si>
   <si>
@@ -255,14 +206,146 @@
     <t>The privacy act appears to relate to government institutions, so it does not appear to have any applicable sections on our program.</t>
   </si>
   <si>
-    <t>s</t>
+    <t>Principle 6 - Accuracy</t>
+  </si>
+  <si>
+    <t>Principle 10 - Challenging Compliance</t>
+  </si>
+  <si>
+    <t>Principle 9 - Individual Access</t>
+  </si>
+  <si>
+    <t>Principle 8 - Openness</t>
+  </si>
+  <si>
+    <t>Principle 7 - Safeguards</t>
+  </si>
+  <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>This is about individuals being able to access their PHI, and the organization having records or the ability to list the organizations that we may have sent PHI to</t>
+  </si>
+  <si>
+    <t>Open about policies and practices related to management of PHI</t>
+  </si>
+  <si>
+    <t>Use of passwords and encryption</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>PHI should be retained only as long as necessary, Develop guideleness and implement procedures w/r to retention of PHI.</t>
+  </si>
+  <si>
+    <t>Only collect necessary PHI</t>
+  </si>
+  <si>
+    <t>Designate an individual / individuals who are accountable for our compliance with the principles</t>
+  </si>
+  <si>
+    <t>N/A - consent is assumed when seeing a HCP</t>
+  </si>
+  <si>
+    <t>https://bccla.org/privacy-handbook/main-menu/privacy8contents/privacy8-2.html#:~:text=In%20most%20cases%20you%20will,because%20your%20consent%20is%20assumed.</t>
+  </si>
+  <si>
+    <t>p. 35</t>
+  </si>
+  <si>
+    <t>Retention of personal info</t>
+  </si>
+  <si>
+    <t>Not for us but states that information must be retained for 1 year if it is used for a decision that affects the patient's health</t>
+  </si>
+  <si>
+    <t>https://laws-lois.justice.gc.ca/eng/acts/p-8.6/</t>
+  </si>
+  <si>
+    <t>Compliance with PIPEDA, Privacy Act, and Personal Information Protection Act</t>
+  </si>
+  <si>
+    <t>PRIVACY ACT</t>
+  </si>
+  <si>
+    <t>PERSONAL INFORMATION PROTECTION</t>
+  </si>
+  <si>
+    <t>See Legal Compliance worksheet</t>
+  </si>
+  <si>
+    <t>use pydicom (library) to convert to .dcm, requires more patient data?</t>
+  </si>
+  <si>
+    <t>RESTful API format, requires more patient data?</t>
+  </si>
+  <si>
+    <t>the 10 PIPEDA principles must be complied with</t>
+  </si>
+  <si>
+    <t>Pairs metadata with pixel data into a .dcm file format, a medical standard, ISO 12052:2017.</t>
+  </si>
+  <si>
+    <t>Standard for exchanging electronic health care data, using an older messaging approach. FHIR is modern HL7 using RESTful APIs</t>
+  </si>
+  <si>
+    <t>hl7apy,python-hl7, fhir.resources, fhirclient, PyFHIR</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>User Guide</t>
+  </si>
+  <si>
+    <t>Data and Privacy Security Guidelines Documentation</t>
+  </si>
+  <si>
+    <t>See Data Privacy and Security Guidelines</t>
+  </si>
+  <si>
+    <r>
+      <t>Documentation outlining how the application handles user data, ensures privacy, and complies with data protection regulations will be provided to inform users about the security measures in place to protect patient information.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>OWASP</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/Django_REST_Framework_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/Django_Security_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/Docker_Security_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <t>test @login_required by using burp suite to send http requests to the backend for the html of pages that should be restricted to authentication users</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/File_Upload_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <t>Below -- Basically "we follow the OWASP cheat sheet series for x, y, and z"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,16 +395,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -329,12 +462,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -344,13 +514,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -393,33 +586,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F9" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
-    <sortCondition ref="A1:A9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:F8" xr:uid="{6E4360FA-3A5F-4CCC-8245-B5ADB39F30B4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
+    <sortCondition ref="A1:A7"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8384FB66-56FA-48BE-BE64-882EF2D985BB}" name="Report Section" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F965AAFA-1C00-4543-93FC-28AD46D0245A}" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F6DA9492-CDDB-4753-8E1F-81D9009A5E9E}" name="Description" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E8E6DE19-837D-4AD6-BB88-8B7F0533BC3D}" name="Feature Specification" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{75DA1F04-D729-4AD5-B1C8-98B285782BD2}" name="Reference" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{E16B3242-CE4B-4B92-8D3C-07721D99D275}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8384FB66-56FA-48BE-BE64-882EF2D985BB}" name="Report Section" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F965AAFA-1C00-4543-93FC-28AD46D0245A}" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{F6DA9492-CDDB-4753-8E1F-81D9009A5E9E}" name="Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E8E6DE19-837D-4AD6-BB88-8B7F0533BC3D}" name="Feature Specification" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{75DA1F04-D729-4AD5-B1C8-98B285782BD2}" name="Reference" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{E16B3242-CE4B-4B92-8D3C-07721D99D275}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79807373-C539-437B-8C4D-7646513B28B3}" name="Table2" displayName="Table2" ref="A2:C9" totalsRowShown="0">
-  <autoFilter ref="A2:C9" xr:uid="{79807373-C539-437B-8C4D-7646513B28B3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C9">
-    <sortCondition ref="A2:A9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6ABD0919-5D52-4949-BD9C-D30A535A992D}" name="Table25" displayName="Table25" ref="A19:C31" totalsRowShown="0">
+  <autoFilter ref="A19:C31" xr:uid="{6ABD0919-5D52-4949-BD9C-D30A535A992D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:B31">
+    <sortCondition ref="A2:A14"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E7B1A1CD-7F3C-445A-A935-DCBB9B3B5494}" name="Section"/>
-    <tableColumn id="2" xr3:uid="{92DFD6EB-9947-474E-8A11-ABE7EBBDC51F}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{241E048F-A3EF-4A2C-8660-987A7CFFFC32}" name="What that means for us"/>
+    <tableColumn id="1" xr3:uid="{873EFAAA-7DFC-47A0-BD7A-06C82DFFD44F}" name="Section" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{332DFBDD-1BD2-4A34-9F27-0E521C4312B1}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{38D9AF5B-0D80-4CCB-BE4C-935FDF0F0C0A}" name="What that means for us" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -742,24 +935,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7F718F-2F7A-4F5E-9A03-E4EADA47E05A}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" customWidth="1"/>
-    <col min="7" max="8" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,143 +969,129 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2.5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
         <v>2.5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
+      <c r="F8" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -926,95 +1105,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEE52AF-1CC7-4463-88B6-73D2896BC707}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="3" max="3" width="75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="L13" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="O13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>4.2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>4.7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>4.8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1023,135 +1403,56 @@
     <hyperlink ref="O13" r:id="rId2" display="https://www.dicomstandard.org/current/" xr:uid="{706AA0A0-063E-4A71-A560-29A7868DE6BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E422045-A429-40C6-BC46-DB83D0D75BA1}">
-  <dimension ref="A1:XFD9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622990F9-57E9-4702-8440-E28BFF890DD9}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="109.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="XFD1" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4.2</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4.3</v>
-      </c>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4.4000000000000004</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>4.5</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3 16384:16384" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FFA380-8EAE-4E77-BE7E-651BA3C1C147}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1159,23 +1460,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DBF29C-7AEC-4AFD-A9AD-8D6FBF1E87A0}">
-  <dimension ref="L20"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9D9303-5F06-48AC-9C60-BA59DB0A294F}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L20" t="s">
-        <v>71</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>